<commit_message>
add MOU from washington dc
</commit_message>
<xml_diff>
--- a/policing_study_contracts/Contracts.xlsx
+++ b/policing_study_contracts/Contracts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericchandler/dev/ucjp-public-data/policing_study_contracts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A3E654-5F84-2046-93F6-0DD3F2F4BDBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF9B25E-E884-9249-A081-E7A4B29CE8A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17600" xr2:uid="{2897005F-A7DB-7A4B-AED2-F3E24885A5EF}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="167">
   <si>
     <t>911 Analysis</t>
   </si>
@@ -522,13 +522,31 @@
   </si>
   <si>
     <t>Contract With</t>
+  </si>
+  <si>
+    <t>DC BWC RCT</t>
+  </si>
+  <si>
+    <t>A randomized control trial evaluating the effects of police body-worn cameras</t>
+  </si>
+  <si>
+    <t>Washington DC</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1073/pnas.1814773116</t>
+  </si>
+  <si>
+    <t>ASU BWC RCT</t>
+  </si>
+  <si>
+    <t>2023-FOIA-08968.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -578,6 +596,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -596,10 +622,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -607,8 +634,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -921,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4221BE9-E742-8E4F-8AEB-C256CC5E36C0}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A3" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1180,7 +1209,7 @@
         <v>81</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>80</v>
@@ -1191,7 +1220,7 @@
         <v>81</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>82</v>
@@ -1202,7 +1231,7 @@
         <v>81</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>83</v>
@@ -1213,7 +1242,7 @@
         <v>81</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>84</v>
@@ -1224,7 +1253,7 @@
         <v>81</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>86</v>
@@ -1235,7 +1264,7 @@
         <v>81</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>89</v>
@@ -1246,7 +1275,7 @@
         <v>81</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>90</v>
@@ -1257,7 +1286,7 @@
         <v>81</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>91</v>
@@ -1268,7 +1297,7 @@
         <v>81</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>92</v>
@@ -1279,7 +1308,7 @@
         <v>81</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>93</v>
@@ -1290,7 +1319,7 @@
         <v>81</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>94</v>
@@ -1301,7 +1330,7 @@
         <v>81</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>95</v>
@@ -1312,7 +1341,7 @@
         <v>81</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>96</v>
@@ -1323,7 +1352,7 @@
         <v>81</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>97</v>
@@ -1334,7 +1363,7 @@
         <v>81</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>98</v>
@@ -1345,7 +1374,7 @@
         <v>81</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>103</v>
@@ -1356,7 +1385,7 @@
         <v>81</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>104</v>
@@ -1367,7 +1396,7 @@
         <v>81</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>105</v>
@@ -1378,7 +1407,7 @@
         <v>81</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>106</v>
@@ -1404,6 +1433,17 @@
       </c>
       <c r="C43" s="5" t="s">
         <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C44" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1418,10 +1458,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BC85F7C-9DCA-FA48-A086-673D22B24751}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1491,7 +1531,7 @@
         <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C6" t="s">
         <v>47</v>
@@ -1502,7 +1542,7 @@
         <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C7" t="s">
         <v>149</v>
@@ -1513,7 +1553,7 @@
         <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C8" t="s">
         <v>52</v>
@@ -1524,7 +1564,7 @@
         <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C9" t="s">
         <v>49</v>
@@ -1535,7 +1575,7 @@
         <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C10" t="s">
         <v>43</v>
@@ -1546,7 +1586,7 @@
         <v>119</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C11" t="s">
         <v>145</v>
@@ -1557,7 +1597,7 @@
         <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="C12" t="s">
         <v>45</v>
@@ -1783,17 +1823,31 @@
         <v>54</v>
       </c>
     </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B33" t="s">
+        <v>161</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C33" r:id="rId1" xr:uid="{9E51DD67-1EEF-7341-A8FA-3426A9DFCA43}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{606EBB6A-158D-6943-9896-89ACAC20AB4E}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1844,7 +1898,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>19</v>
@@ -1959,6 +2013,14 @@
         <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>161</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1969,10 +2031,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6AD3E6-8C5E-E343-A99E-0C1105DA298B}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2348,6 +2410,14 @@
         <v>158</v>
       </c>
     </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>162</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>